<commit_message>
idfk; but Table Grouping works now
</commit_message>
<xml_diff>
--- a/data/xlsx_edit/physrostr17.xlsx
+++ b/data/xlsx_edit/physrostr17.xlsx
@@ -2912,8 +2912,8 @@
   </sheetPr>
   <dimension ref="A1:O791"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A757" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I769" activeCellId="0" sqref="I769"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F47" activeCellId="0" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4299,7 +4299,7 @@
         <v>33</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>488</v>
+        <v>2488</v>
       </c>
       <c r="G46" s="2" t="n">
         <v>0</v>

</xml_diff>